<commit_message>
Update journal / websummary
</commit_message>
<xml_diff>
--- a/documentation/Jules/3_1_Journal_Jules.xlsx
+++ b/documentation/Jules/3_1_Journal_Jules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/jules_crausaz_studentfr_ch/Documents/EMF/3eme/306/306-G3-SpeleoThink/documentation/Jules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69245CCB-C41C-46A9-B8A7-7CF778EA1619}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC83C5E-415E-4F16-98EE-FA387BE807BD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>Je trouve que le groupe fonctionne très bien et la répartition des tâches se fait très bien. Le reste de l'après midi je n'étais pas là, car j'ai été me faire retirer les dents de sagesse.</t>
+  </si>
+  <si>
+    <t>finalisaion des maquettes ainsi que l'ajout des maquette dans la documentation</t>
+  </si>
+  <si>
+    <t>Commencement du web summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je trouve que le groupe fonctionne très bien. La répartition à bien été effectuée. </t>
   </si>
 </sst>
 </file>
@@ -522,100 +531,100 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -898,6 +907,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1251,9 +1264,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
+      <selection pane="bottomLeft" activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1266,85 +1279,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34">
+      <c r="A6" s="20">
         <v>45996</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1357,67 +1370,67 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
+      <c r="A13" s="29">
         <v>46003</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="20"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1430,59 +1443,59 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
+      <c r="A20" s="29">
         <v>46009</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1495,67 +1508,67 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14">
+      <c r="A27" s="29">
         <v>46010</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="31"/>
       <c r="D27" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="19" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="19" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="20"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1568,53 +1581,53 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="32"/>
+      <c r="B33" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
+      <c r="A34" s="29">
         <v>46030</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="18"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="19" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="20"/>
+      <c r="C35" s="25"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1627,49 +1640,49 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="21" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14">
+      <c r="A41" s="29">
         <v>46031</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="18"/>
+      <c r="C41" s="31"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="20"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="25"/>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1682,47 +1695,55 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
-      <c r="B47" s="21" t="s">
+      <c r="A47" s="32"/>
+      <c r="B47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="23"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14">
+      <c r="A48" s="29">
         <v>15.012600000000001</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="31"/>
+      <c r="D48" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="8"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1731,47 +1752,49 @@
       </c>
       <c r="D53" s="9">
         <f>SUM(D48:D52)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="23"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="34"/>
+      <c r="D54" s="35"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="18"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="20"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="25"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="20"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="25"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="20"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="25"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="20"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1784,43 +1807,43 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="16"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="23"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="35"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="18"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="25"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="25"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="20"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="15"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1833,43 +1856,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="26"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="28"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="18"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="31"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="15"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="20"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="25"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="15"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="25"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1882,43 +1905,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="16"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="23"/>
+      <c r="A75" s="32"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="35"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="18"/>
+      <c r="A76" s="29"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="31"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="15"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="20"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="25"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="25"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="25"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1931,10 +1954,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="16"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="23"/>
+      <c r="A82" s="32"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="35"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1944,19 +1967,90 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>21.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -1968,77 +2062,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2162,17 +2185,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2385,6 +2397,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
@@ -2394,19 +2417,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2423,4 +2433,17 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>